<commit_message>
LCA all wave, pooled, differences in sums for chronic conditions and CAMs
</commit_message>
<xml_diff>
--- a/R/complete4StatesCondProb.xlsx
+++ b/R/complete4StatesCondProb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanna\Documents\git\AHL\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17011909-C0FA-460C-ABC6-B02BA694F768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C50B67-6E3F-4409-A6C4-ED2F36E39391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -459,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" zoomScale="127" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>